<commit_message>
mise à jour du site web
</commit_message>
<xml_diff>
--- a/pdf/Tableau.xlsx
+++ b/pdf/Tableau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\Portfolio\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295F54DF-B1A0-431B-927D-2FF4E8C2F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B335AC6-9C02-437E-A32C-C28141E80EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -109,9 +109,6 @@
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t>SESSION 2022</t>
-  </si>
-  <si>
     <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>13/09/22 au 06/01/23</t>
   </si>
   <si>
-    <t>27/01/22 au 07/02/23</t>
-  </si>
-  <si>
     <t>Mise en place d'un CXR et d'un Opengear (voir page projets pro de mon portfolio)</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>Réalisation de chemins de câble via un fichier d'audit de locaux techniques pour l'installation d'un appareil de prise en main à distance sur les ports consoles  (fichier sur portfolio + cahier de stage)</t>
+  </si>
+  <si>
+    <t>27/01/22 au 16/03/23</t>
+  </si>
+  <si>
+    <t>SESSION 2023</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
   </sheetPr>
   <dimension ref="A1:AQ75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="71" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -986,7 +986,7 @@
       <c r="E1" s="18"/>
       <c r="F1" s="18"/>
       <c r="G1" s="18" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="H1" s="18"/>
     </row>
@@ -1004,14 +1004,14 @@
     </row>
     <row r="3" spans="1:43" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
       <c r="E3" s="29"/>
       <c r="F3" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="29"/>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="4" spans="1:43" ht="40.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
@@ -1031,7 +1031,7 @@
         <v>8</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="13" t="s">
         <v>15</v>
@@ -1042,7 +1042,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>0</v>
@@ -1169,13 +1169,13 @@
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="15" t="s">
-        <v>36</v>
-      </c>
       <c r="C8" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1220,13 +1220,13 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -1271,14 +1271,14 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1322,20 +1322,20 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1375,10 +1375,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -1386,7 +1386,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1426,19 +1426,21 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="H13" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1477,17 +1479,17 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14"/>
@@ -1528,10 +1530,10 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -1539,7 +1541,7 @@
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1579,15 +1581,15 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1630,7 +1632,7 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -1677,13 +1679,13 @@
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>38</v>
-      </c>
       <c r="C18" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -1728,21 +1730,21 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19"/>
@@ -1783,13 +1785,13 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="C20" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -1834,19 +1836,19 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21" s="14"/>
       <c r="I21"/>
@@ -1887,17 +1889,17 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H22" s="14"/>
       <c r="I22"/>
@@ -1938,21 +1940,21 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="14"/>
       <c r="I23"/>
@@ -1993,7 +1995,7 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -2040,17 +2042,17 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="15" t="s">
         <v>42</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>44</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25"/>
@@ -2091,23 +2093,23 @@
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H26" s="14"/>
       <c r="I26"/>
@@ -2148,21 +2150,21 @@
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H27" s="14"/>
       <c r="I27"/>
@@ -2203,20 +2205,20 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -2364,7 +2366,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="49" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="36" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>